<commit_message>
add metadata for damage type observed
</commit_message>
<xml_diff>
--- a/metadata/JRBPmidAprPathPrcntDamCulturesData_25Apr2015ERS_metadata.xlsx
+++ b/metadata/JRBPmidAprPathPrcntDamCulturesData_25Apr2015ERS_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AmyKendig/Google Drive/JRBP Project/invasion-pathogen-communities/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DCE075E-1360-A64A-847C-4E5935E94BD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3D523A-4EDB-D24B-B1BC-6EBF421BF16D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11060" yWindow="980" windowWidth="27240" windowHeight="16440" xr2:uid="{27A6BE13-21EA-3240-9134-F037E2CFD48E}"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="27240" windowHeight="16440" xr2:uid="{27A6BE13-21EA-3240-9134-F037E2CFD48E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t>observer</t>
   </si>
@@ -125,13 +125,19 @@
     <t>a unique plant identification</t>
   </si>
   <si>
-    <t>disease severity score for one of out up to six leaves per plant (percentage of leaf surface area covered with lesions)</t>
-  </si>
-  <si>
     <t>initials of person who recorded disease severity assessment</t>
   </si>
   <si>
     <t>identification number for tissue sample collected</t>
+  </si>
+  <si>
+    <t>disease severity score for one of up to six leaves per plant (percentage of leaf surface area covered with lesions)</t>
+  </si>
+  <si>
+    <t>damage type observed (DTO) for one of up to sixe leaves per plant (see KeyDamageTypesJRBPGrasses_SpearMar2015.pdf in metadata for key)</t>
+  </si>
+  <si>
+    <t>damage type observed (DTO) for tissue sample collected (see KeyDamageTypesJRBPGrasses_SpearMar2015.pdf in metadata for key)</t>
   </si>
 </sst>
 </file>
@@ -486,7 +492,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -512,7 +518,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -560,90 +566,111 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>